<commit_message>
finally commit what I did before going on leave
</commit_message>
<xml_diff>
--- a/support/IndicatorInformation.xlsx
+++ b/support/IndicatorInformation.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JonMinton/repos/mhi-cyp-backend/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3016F58-F419-3444-BA59-D212863B4260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82721C39-250A-A343-9DB9-4201EB0229A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{F5096571-3C68-2847-9195-676E70D8D131}"/>
+    <workbookView minimized="1" xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{F5096571-3C68-2847-9195-676E70D8D131}"/>
   </bookViews>
   <sheets>
     <sheet name="all_indicators" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_indicators!$A$1:$H$71</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -368,9 +371,6 @@
     <t>Percentage of P7-S3 pupils who report having never been cyber bullied</t>
   </si>
   <si>
-    <t>Learning environment</t>
-  </si>
-  <si>
     <t>Engagement with learning</t>
   </si>
   <si>
@@ -380,9 +380,6 @@
     <t>Percentage school attendance by primary and secondary pupils in the past year</t>
   </si>
   <si>
-    <t>Scottosh Government School Statistics</t>
-  </si>
-  <si>
     <t>Liking school</t>
   </si>
   <si>
@@ -630,6 +627,12 @@
   </si>
   <si>
     <t>Scottish Government Social Work Statistics</t>
+  </si>
+  <si>
+    <t>Scottish Government School Statistics</t>
+  </si>
+  <si>
+    <t>Learning Environment</t>
   </si>
 </sst>
 </file>
@@ -999,8 +1002,8 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2087,22 +2090,22 @@
         <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D42" t="s">
         <v>110</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G42" t="b">
         <v>0</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>114</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -2113,16 +2116,16 @@
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D43" t="s">
         <v>110</v>
       </c>
-      <c r="D43" t="s">
-        <v>111</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -2139,16 +2142,16 @@
         <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="D44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
@@ -2165,16 +2168,16 @@
         <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="D45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
@@ -2191,16 +2194,16 @@
         <v>4</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="D46" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
@@ -2217,16 +2220,16 @@
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="D47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -2243,16 +2246,16 @@
         <v>4</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -2269,16 +2272,16 @@
         <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D49" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F49" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -2295,16 +2298,16 @@
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
@@ -2321,16 +2324,16 @@
         <v>4</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
@@ -2347,16 +2350,16 @@
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D52" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -2373,16 +2376,16 @@
         <v>4</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="G53" t="b">
         <v>1</v>
@@ -2399,22 +2402,22 @@
         <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" t="s">
+        <v>144</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F54" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G54" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -2425,22 +2428,22 @@
         <v>4</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D55" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="G55" t="b">
         <v>0</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -2451,22 +2454,22 @@
         <v>4</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D56" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G56" t="b">
-        <v>0</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -2477,22 +2480,22 @@
         <v>4</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -2503,16 +2506,16 @@
         <v>4</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
@@ -2529,22 +2532,22 @@
         <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G59" t="b">
-        <v>0</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -2555,22 +2558,22 @@
         <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D60" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -2581,22 +2584,22 @@
         <v>4</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G61" t="b">
-        <v>0</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -2607,22 +2610,22 @@
         <v>4</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G62" t="b">
-        <v>0</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -2633,22 +2636,22 @@
         <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D63" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G63" t="b">
-        <v>0</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -2659,16 +2662,16 @@
         <v>4</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D64" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="G64" t="b">
         <v>1</v>
@@ -2685,16 +2688,16 @@
         <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2711,16 +2714,16 @@
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D66" t="s">
+        <v>178</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
@@ -2737,16 +2740,16 @@
         <v>4</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G67" t="b">
         <v>1</v>
@@ -2763,22 +2766,22 @@
         <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D68" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E68" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G68" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -2789,16 +2792,16 @@
         <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D69" t="s">
+        <v>186</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="G69" t="b">
         <v>1</v>
@@ -2815,22 +2818,22 @@
         <v>4</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D70" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G70" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -2841,25 +2844,26 @@
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D71" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E71" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G71" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>197</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H71" xr:uid="{6A8A637E-34F8-A941-AE31-C63F861ABD7F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>